<commit_message>
Added paths for preloaded image list.
</commit_message>
<xml_diff>
--- a/Counterbalancing planning.xlsx
+++ b/Counterbalancing planning.xlsx
@@ -1347,7 +1347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F86428-05F7-7542-9223-34A7B4EC2D35}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9571,7 +9573,7 @@
         <v>PICTURES/filler-foods/taco.jpeg</v>
       </c>
       <c r="F3" s="8" t="str">
-        <f t="shared" ref="F3:F49" si="0">_xlfn.CONCAT("You look at a ",C3,".")</f>
+        <f t="shared" ref="F3:F48" si="0">_xlfn.CONCAT("You look at a ",C3,".")</f>
         <v>You look at a taco.</v>
       </c>
       <c r="G3" s="15" t="s">
@@ -9755,7 +9757,7 @@
         <v>222</v>
       </c>
       <c r="H10" s="8" t="str">
-        <f t="shared" ref="H10:H25" si="1">I11</f>
+        <f t="shared" ref="H10:H24" si="1">I11</f>
         <v>PICTURES/filler-foods/cracker.jpeg</v>
       </c>
       <c r="I10" s="8" t="s">

</xml_diff>